<commit_message>
Update coding convention, case breaking new line while coding.
</commit_message>
<xml_diff>
--- a/Support/Coding Convention.xlsx
+++ b/Support/Coding Convention.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <r>
       <t xml:space="preserve">Tất cả Business Code Logic được đặt trong </t>
@@ -1050,6 +1050,25 @@
       </rPr>
       <t>Async</t>
     </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Trong trường hợp cần xuống hàng vì </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Code quá dài</t>
+    </r>
+  </si>
+  <si>
+    <t>thì nên xuống hàng tại vị trí của toán tử, hoặc sau dấu chấm</t>
   </si>
 </sst>
 </file>
@@ -1739,6 +1758,50 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>151</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>171450</xdr:colOff>
+      <xdr:row>160</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId15">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="28765500"/>
+          <a:ext cx="2000250" cy="1800225"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -2005,9 +2068,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B131"/>
+  <dimension ref="A1:B151"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G158" sqref="G158"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -2157,6 +2222,19 @@
         <v>22</v>
       </c>
     </row>
+    <row r="150" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A150" s="1">
+        <v>11</v>
+      </c>
+      <c r="B150" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="151" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B151" t="s">
+        <v>24</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>